<commit_message>
Sixt als Sponsor ?
</commit_message>
<xml_diff>
--- a/Marketing/Sponsorenliste.xlsx
+++ b/Marketing/Sponsorenliste.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GRUBERT\Documents\COSIMA-Laserstar\Marketing\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="6255"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="6260"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="117">
   <si>
     <t>Website</t>
   </si>
@@ -366,13 +361,22 @@
   </si>
   <si>
     <t>Anfrage gesendet</t>
+  </si>
+  <si>
+    <t>Sixt GmbH &amp; Co. Autovermietung KG</t>
+  </si>
+  <si>
+    <t>kundenbetreuung@sixt.com</t>
+  </si>
+  <si>
+    <t>089 744440</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -493,7 +497,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -552,7 +556,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -604,7 +608,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -798,37 +802,37 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A47" sqref="A46:A47"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
-    <col min="3" max="3" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.453125" customWidth="1"/>
+    <col min="3" max="3" width="38.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -848,7 +852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -863,7 +867,7 @@
       </c>
       <c r="M4" s="9"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
@@ -881,7 +885,7 @@
       </c>
       <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="9" t="s">
         <v>14</v>
       </c>
@@ -893,7 +897,7 @@
       </c>
       <c r="M6" s="9"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="9" t="s">
         <v>15</v>
       </c>
@@ -905,7 +909,7 @@
       </c>
       <c r="M7" s="9"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="9" t="s">
         <v>16</v>
       </c>
@@ -914,7 +918,7 @@
       </c>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="8" t="s">
         <v>17</v>
       </c>
@@ -931,7 +935,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="5" customFormat="1">
       <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
@@ -945,7 +949,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="5" customFormat="1" ht="43.5">
       <c r="A11" s="14" t="s">
         <v>25</v>
       </c>
@@ -962,7 +966,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="43.5">
       <c r="A12" s="8" t="s">
         <v>30</v>
       </c>
@@ -979,7 +983,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="5" customFormat="1">
       <c r="A13" s="5" t="s">
         <v>22</v>
       </c>
@@ -996,7 +1000,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="5" customFormat="1">
       <c r="B14" s="5" t="s">
         <v>38</v>
       </c>
@@ -1007,7 +1011,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="5" customFormat="1">
       <c r="C15" s="6" t="s">
         <v>41</v>
       </c>
@@ -1015,7 +1019,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="43.5">
       <c r="A16" s="8" t="s">
         <v>42</v>
       </c>
@@ -1041,7 +1045,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="43.5">
       <c r="A17" s="8" t="s">
         <v>47</v>
       </c>
@@ -1064,7 +1068,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="43.5">
       <c r="A18" s="8" t="s">
         <v>57</v>
       </c>
@@ -1084,7 +1088,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13">
       <c r="A19" s="9" t="s">
         <v>69</v>
       </c>
@@ -1092,7 +1096,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="A23" s="9" t="s">
         <v>71</v>
       </c>
@@ -1103,7 +1107,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="29">
       <c r="A24" s="9" t="s">
         <v>75</v>
       </c>
@@ -1117,16 +1121,16 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" s="7" customFormat="1">
       <c r="B25" s="12"/>
       <c r="C25" s="13"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13">
       <c r="A26" s="9" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13">
       <c r="A27" s="8" t="s">
         <v>79</v>
       </c>
@@ -1137,7 +1141,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" s="5" customFormat="1">
       <c r="A28" s="16" t="s">
         <v>80</v>
       </c>
@@ -1148,7 +1152,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" s="4" customFormat="1">
       <c r="A29" s="17" t="s">
         <v>85</v>
       </c>
@@ -1162,7 +1166,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" s="5" customFormat="1">
       <c r="A30" s="16" t="s">
         <v>88</v>
       </c>
@@ -1176,7 +1180,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" s="4" customFormat="1" ht="43.5">
       <c r="A31" s="18" t="s">
         <v>93</v>
       </c>
@@ -1196,7 +1200,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" s="5" customFormat="1">
       <c r="A32" s="16" t="s">
         <v>99</v>
       </c>
@@ -1213,7 +1217,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" s="4" customFormat="1">
       <c r="A33" s="18" t="s">
         <v>104</v>
       </c>
@@ -1230,7 +1234,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" s="4" customFormat="1">
       <c r="A34" s="17" t="s">
         <v>105</v>
       </c>
@@ -1244,30 +1248,41 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" s="4" customFormat="1">
       <c r="A35" s="18" t="s">
         <v>111</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D35"/>
       <c r="F35"/>
     </row>
-    <row r="36" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
-      <c r="D36"/>
+    <row r="36" spans="1:6" s="4" customFormat="1">
+      <c r="A36" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" t="s">
+        <v>116</v>
+      </c>
       <c r="F36"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="B38" t="s">
+    <row r="37" spans="1:6" s="4" customFormat="1">
+      <c r="A37" s="17"/>
+      <c r="D37"/>
+      <c r="F37"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="8"/>
+      <c r="B39" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
-      <c r="B39" t="s">
+    <row r="40" spans="1:6">
+      <c r="A40" s="9"/>
+      <c r="B40" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1294,8 +1309,9 @@
     <hyperlink ref="C24" r:id="rId19" display="info@cki.rwth-aachen.de/Marina Brandt"/>
     <hyperlink ref="C27" r:id="rId20"/>
     <hyperlink ref="C33" r:id="rId21"/>
+    <hyperlink ref="C36" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>